<commit_message>
updating for joust functionality
</commit_message>
<xml_diff>
--- a/Homework/ArcadeGame/final_functionality_worksheet.xlsx
+++ b/Homework/ArcadeGame/final_functionality_worksheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t xml:space="preserve">Team Number:</t>
   </si>
@@ -64,28 +64,28 @@
     <t xml:space="preserve">A hero that can move</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumping and correctly standing on platforms with gravity</t>
+    <t xml:space="preserve">Jumping and correctly standing on platforms with gravity, no getting stuck or weirdness</t>
   </si>
   <si>
     <t xml:space="preserve">Switching between levels with U and D and when defeating monsters</t>
   </si>
   <si>
-    <t xml:space="preserve">Moving monsters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monsters killing the hero, appropiate use of lives and final game over</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Player shoots bubbles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monsters trapped by bubbles, float to the top of the screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shooting monster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score tracking, Fruit that appears from bubbles</t>
+    <t xml:space="preserve">Moving monsters, flying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset on death, appropiate use of lives and final game over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct player/monster jousting behavior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eggs dropping, pickup by hero, and becoming monsters if not picked up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shooting monster/bullet behavior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score tracking, increases on eggs (and maybe other things)</t>
   </si>
   <si>
     <t xml:space="preserve">Other functionalities in the basic game</t>
@@ -97,10 +97,22 @@
     <t xml:space="preserve">Extra Functionality:</t>
   </si>
   <si>
+    <t xml:space="preserve">APPROX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suggestions from spec</t>
   </si>
   <si>
-    <t xml:space="preserve">Images for the player, monsters, environment, power-ups</t>
+    <t xml:space="preserve">Images, more if animated or correctly do directions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music/sound, more if effects integrated with a lot of different events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-5</t>
   </si>
   <si>
     <t xml:space="preserve">Even more qualitatively different kinds of enemies</t>
@@ -118,13 +130,10 @@
     <t xml:space="preserve">Help screen that explains the keys (this is a minor one)</t>
   </si>
   <si>
-    <t xml:space="preserve">Basic start screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animated start screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boss fight level where you must defeat a giant enemy</t>
+    <t xml:space="preserve">Basic start screen, more if animated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boss</t>
   </si>
   <si>
     <t xml:space="preserve">List others here:</t>
@@ -133,7 +142,13 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t xml:space="preserve">* Note that the main guidance for extra functional is 21 points is approximately 1 milestone worth of work.  These point values are very general guidance.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> TOTAL POINTS FOR EXTRA FUNCTIONALITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra Credit points</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL POINTS</t>
@@ -146,9 +161,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -196,7 +212,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +229,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDCE6F2"/>
         <bgColor rgb="FFD7E4BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -279,7 +301,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -299,7 +321,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -311,10 +333,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,7 +345,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -334,18 +356,18 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -367,7 +389,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFDCE6F2"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -417,17 +439,17 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="100.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="8.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="8.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -536,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="11" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
@@ -606,7 +628,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="11" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12"/>
@@ -651,101 +673,119 @@
       <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="C26" s="17"/>
       <c r="D26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="0"/>
       <c r="C27" s="11"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="C28" s="11"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="C29" s="11"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="B30" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="C30" s="11"/>
       <c r="D30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="B31" s="11" t="n">
+        <v>5</v>
+      </c>
       <c r="C31" s="11"/>
       <c r="D31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="B32" s="11" t="n">
+        <v>6</v>
+      </c>
       <c r="C32" s="11"/>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="C33" s="11"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="B34" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="C34" s="11"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="C35" s="11"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="C36" s="11"/>
       <c r="D36" s="12"/>
     </row>
     <row r="37" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
-        <v>36</v>
+      <c r="A38" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -753,7 +793,7 @@
     </row>
     <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -761,23 +801,23 @@
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="12"/>
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="s">
-        <v>36</v>
+      <c r="A41" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
       <c r="D41" s="12"/>
     </row>
-    <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
-        <v>36</v>
+    <row r="42" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -785,60 +825,72 @@
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="D43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="14" t="n">
+      <c r="A44" s="0"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="C44" s="14" t="n">
-        <f aca="false">SUM(C27:C43)</f>
+      <c r="C45" s="14" t="n">
+        <f aca="false">SUM(C27:C44)</f>
         <v>0</v>
       </c>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="16"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
+      <c r="D45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="16"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
+      <c r="A46" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="C46" s="11" t="n">
+        <f aca="false">MIN(MAX(C45-B45,0)*0.5, B46)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="7" t="n">
-        <f aca="false">SUM(B24,B44)</f>
+      <c r="A47" s="16"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="7" t="n">
+        <f aca="false">SUM(B24,B45)</f>
         <v>140</v>
       </c>
-      <c r="C47" s="7" t="n">
-        <f aca="false">SUM(C24,C44)</f>
+      <c r="C48" s="7" t="n">
+        <f aca="false">SUM(C24,C45)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D50" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D53" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D51" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D54" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>